<commit_message>
Updated budget a bit
</commit_message>
<xml_diff>
--- a/budget/CZI HCA Goff Budget 2017 Draft.xlsx
+++ b/budget/CZI HCA Goff Budget 2017 Draft.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$62</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$59</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Personnel:</t>
   </si>
@@ -79,15 +79,6 @@
   </si>
   <si>
     <t>Reagents for enzymatic dissociation of single cells and seq. library preparation</t>
-  </si>
-  <si>
-    <t>Elana Fertig</t>
-  </si>
-  <si>
-    <t>Co-Investigator</t>
-  </si>
-  <si>
-    <t>Seth Blackshaw</t>
   </si>
   <si>
     <t>Services</t>
@@ -1129,10 +1120,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1151,7 +1142,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="70" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="28"/>
@@ -1195,7 +1186,7 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" s="7">
         <v>130050</v>
@@ -1222,233 +1213,215 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D4" s="66">
-        <v>119100</v>
+        <v>0</v>
       </c>
       <c r="E4" s="67">
-        <f t="shared" ref="E4:E11" si="0">12*F4</f>
-        <v>1.7999999999999998</v>
+        <v>0</v>
       </c>
       <c r="F4" s="68">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="G4" s="10">
-        <f t="shared" ref="G4:G11" si="1">D4*F4</f>
-        <v>17865</v>
+        <v>0</v>
       </c>
       <c r="H4" s="10">
-        <f t="shared" ref="H4" si="2">G4*0.34</f>
-        <v>6074.1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="37">
-        <f t="shared" ref="I4:I7" si="3">SUM(G4:H4)</f>
-        <v>23939.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="66">
-        <v>165000</v>
+        <v>47853</v>
       </c>
       <c r="E5" s="67">
-        <f t="shared" si="0"/>
-        <v>1.2000000000000002</v>
+        <f t="shared" ref="E5:E8" si="0">12*F5</f>
+        <v>12</v>
       </c>
       <c r="F5" s="68">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="G5" s="10">
-        <f>D5*F5</f>
-        <v>16500</v>
+        <f t="shared" ref="G5:G8" si="1">D5*F5</f>
+        <v>47853</v>
       </c>
       <c r="H5" s="10">
-        <f>G5*0.34</f>
-        <v>5610</v>
+        <f>G5*0.193</f>
+        <v>9235.6290000000008</v>
       </c>
       <c r="I5" s="37">
-        <f t="shared" si="3"/>
-        <v>22110</v>
+        <f t="shared" ref="I5" si="2">SUM(G5:H5)</f>
+        <v>57088.629000000001</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>32</v>
+      <c r="A6" s="49" t="s">
+        <v>13</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="6" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D6" s="66">
-        <v>0</v>
+        <v>47853</v>
       </c>
       <c r="E6" s="67">
-        <v>0</v>
+        <f t="shared" ref="E6" si="3">12*F6</f>
+        <v>6</v>
       </c>
       <c r="F6" s="68">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G6" s="10">
-        <v>0</v>
+        <f t="shared" ref="G6" si="4">D6*F6</f>
+        <v>23926.5</v>
       </c>
       <c r="H6" s="10">
-        <v>0</v>
+        <f>G6*0.193</f>
+        <v>4617.8145000000004</v>
       </c>
       <c r="I6" s="37">
-        <v>0</v>
+        <f t="shared" ref="I6" si="5">SUM(G6:H6)</f>
+        <v>28544.3145</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="66">
-        <v>47853</v>
-      </c>
-      <c r="E7" s="67">
+        <v>12</v>
+      </c>
+      <c r="D7" s="7">
+        <v>33000</v>
+      </c>
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="F7" s="68">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.5</v>
       </c>
       <c r="G7" s="10">
         <f t="shared" si="1"/>
-        <v>47853</v>
+        <v>16500</v>
       </c>
       <c r="H7" s="10">
-        <f>G7*0.193</f>
-        <v>9235.6290000000008</v>
+        <f>G7*0</f>
+        <v>0</v>
       </c>
       <c r="I7" s="37">
-        <f t="shared" si="3"/>
-        <v>57088.629000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="49"/>
+        <f>SUM(G7:H7)</f>
+        <v>16500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="37"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="37"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E10" s="8">
+      <c r="C8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="7">
+        <v>34000</v>
+      </c>
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F8" s="9">
         <v>0.5</v>
       </c>
-      <c r="G10" s="10">
-        <f t="shared" si="1"/>
-        <v>16500</v>
-      </c>
-      <c r="H10" s="10">
-        <f>G10*0</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="37">
-        <f>SUM(G10:H10)</f>
-        <v>16500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="7">
-        <v>34000</v>
-      </c>
-      <c r="E11" s="8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G11" s="10">
+      <c r="G8" s="10">
         <f t="shared" si="1"/>
         <v>17000</v>
       </c>
-      <c r="H11" s="10">
-        <f t="shared" ref="H11" si="4">G11*0.34</f>
+      <c r="H8" s="10">
+        <f t="shared" ref="H8" si="6">G8*0.34</f>
         <v>5780</v>
       </c>
-      <c r="I11" s="37">
-        <f>SUM(G11:H11)</f>
+      <c r="I8" s="37">
+        <f>SUM(G8:H8)</f>
         <v>22780</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+    <row r="9" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13">
-        <f>SUM(G3:G11)</f>
-        <v>141728</v>
-      </c>
-      <c r="H12" s="13">
-        <f>SUM(H3:H11)</f>
-        <v>35543.129000000001</v>
-      </c>
-      <c r="I12" s="38">
-        <f>SUM(I3:I11)</f>
-        <v>177271.12900000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
-      <c r="B13" s="75"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13">
+        <f>SUM(G3:G8)</f>
+        <v>131289.5</v>
+      </c>
+      <c r="H9" s="13">
+        <f>SUM(H3:H8)</f>
+        <v>28476.843500000003</v>
+      </c>
+      <c r="I9" s="38">
+        <f>SUM(I3:I8)</f>
+        <v>159766.34350000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="39"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="39"/>
+    </row>
+    <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="39"/>
+    </row>
+    <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="71"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -1458,8 +1431,10 @@
       <c r="I13" s="39"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="75"/>
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="24"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -1468,46 +1443,55 @@
       <c r="H14" s="16"/>
       <c r="I14" s="39"/>
     </row>
-    <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="71" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="39"/>
-    </row>
-    <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="71"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="39"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="48">
+        <f>2*21000</f>
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="43">
+        <v>1440</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="39"/>
+      <c r="A17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="43">
+        <v>805</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1516,14 +1500,11 @@
       <c r="F18" s="4"/>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
-      <c r="I18" s="48">
-        <f>2*21000</f>
-        <v>42000</v>
-      </c>
+      <c r="I18" s="43"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1532,13 +1513,11 @@
       <c r="F19" s="4"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
-      <c r="I19" s="43">
-        <v>1440</v>
-      </c>
+      <c r="I19" s="43"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1547,51 +1526,53 @@
       <c r="F20" s="4"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
-      <c r="I20" s="43">
-        <v>805</v>
-      </c>
+      <c r="I20" s="43"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
       <c r="I21" s="43"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="43"/>
+        <v>15</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="43">
+        <v>3500</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="43"/>
+        <v>19</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="37">
+        <v>5315</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
@@ -1599,27 +1580,23 @@
       <c r="F24" s="15"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
-      <c r="I24" s="43"/>
+      <c r="I24" s="37">
+        <v>5500</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="43">
-        <v>3500</v>
-      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="37"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
@@ -1627,13 +1604,11 @@
       <c r="F26" s="15"/>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
-      <c r="I26" s="37">
-        <v>5315</v>
-      </c>
+      <c r="I26" s="37"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>14</v>
+      <c r="A27" s="25" t="s">
+        <v>16</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -1642,23 +1617,26 @@
       <c r="F27" s="15"/>
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
-      <c r="I27" s="37">
-        <v>5500</v>
-      </c>
+      <c r="I27" s="37"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
+      <c r="A28" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="37"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="37">
+        <f>16*2000</f>
+        <v>32000</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
+      <c r="A29" s="4"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
@@ -1670,7 +1648,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="25" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -1683,7 +1661,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -1693,12 +1671,13 @@
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
       <c r="I31" s="37">
-        <f>16*2000</f>
-        <v>32000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
+      <c r="A32" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
@@ -1706,177 +1685,175 @@
       <c r="F32" s="15"/>
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
-      <c r="I32" s="37"/>
+      <c r="I32" s="37">
+        <v>5000</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="25" t="s">
-        <v>29</v>
-      </c>
+      <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
       <c r="I33" s="37"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="37">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="37">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
+    <row r="34" spans="1:9" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="37"/>
+    </row>
+    <row r="35" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="38">
+        <f>SUM(I15:I34)</f>
+        <v>99060</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
       <c r="I36" s="37"/>
     </row>
-    <row r="37" spans="1:9" s="22" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="76"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="37"/>
-    </row>
-    <row r="38" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="38">
-        <f>SUM(I18:I37)</f>
-        <v>99060</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="37"/>
-    </row>
-    <row r="40" spans="1:9" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="73" t="s">
+    <row r="37" spans="1:9" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="40">
-        <f>(I38+I12)</f>
-        <v>276331.12900000002</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="72"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="39"/>
-    </row>
-    <row r="42" spans="1:9" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="H42" s="44">
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="40">
+        <f>(I35+I9)</f>
+        <v>258826.34350000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="72"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="39"/>
+    </row>
+    <row r="39" spans="1:9" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="29"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" s="44">
         <v>0.15</v>
       </c>
-      <c r="I42" s="46">
-        <f>I40*H42</f>
-        <v>41449.669350000004</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B43" s="30"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="41">
-        <f>I42+I40</f>
-        <v>317780.79835</v>
-      </c>
+      <c r="I39" s="46">
+        <f>I37*H39</f>
+        <v>38823.951525000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="30"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="41">
+        <f>I39+I37</f>
+        <v>297650.295025</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="51"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="56"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="57"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="59"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="61"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="59"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="59"/>
+      <c r="H43" s="59"/>
+      <c r="I43" s="61"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="50" t="s">
+      <c r="A44" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="51"/>
-      <c r="C44" s="52"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="57"/>
+      <c r="B44" s="59"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="61"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="58" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B45" s="59"/>
       <c r="C45" s="60"/>
@@ -1928,7 +1905,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="58" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B49" s="59"/>
       <c r="C49" s="60"/>
@@ -1941,7 +1918,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="58" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B50" s="59"/>
       <c r="C50" s="60"/>
@@ -1953,9 +1930,7 @@
       <c r="I50" s="61"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="58" t="s">
-        <v>41</v>
-      </c>
+      <c r="A51" s="58"/>
       <c r="B51" s="59"/>
       <c r="C51" s="60"/>
       <c r="D51" s="59"/>
@@ -1966,8 +1941,8 @@
       <c r="I51" s="61"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="58" t="s">
-        <v>43</v>
+      <c r="A52" s="69" t="s">
+        <v>32</v>
       </c>
       <c r="B52" s="59"/>
       <c r="C52" s="60"/>
@@ -1980,7 +1955,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="58" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B53" s="59"/>
       <c r="C53" s="60"/>
@@ -1992,7 +1967,9 @@
       <c r="I53" s="61"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="58"/>
+      <c r="A54" s="58" t="s">
+        <v>43</v>
+      </c>
       <c r="B54" s="59"/>
       <c r="C54" s="60"/>
       <c r="D54" s="59"/>
@@ -2003,8 +1980,8 @@
       <c r="I54" s="61"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="69" t="s">
-        <v>35</v>
+      <c r="A55" s="58" t="s">
+        <v>44</v>
       </c>
       <c r="B55" s="59"/>
       <c r="C55" s="60"/>
@@ -2055,54 +2032,15 @@
       <c r="I58" s="61"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="B59" s="59"/>
-      <c r="C59" s="60"/>
-      <c r="D59" s="59"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="59"/>
-      <c r="G59" s="59"/>
-      <c r="H59" s="59"/>
-      <c r="I59" s="61"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="B60" s="59"/>
-      <c r="C60" s="60"/>
-      <c r="D60" s="59"/>
-      <c r="E60" s="59"/>
-      <c r="F60" s="59"/>
-      <c r="G60" s="59"/>
-      <c r="H60" s="59"/>
-      <c r="I60" s="61"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="B61" s="59"/>
-      <c r="C61" s="60"/>
-      <c r="D61" s="59"/>
-      <c r="E61" s="59"/>
-      <c r="F61" s="59"/>
-      <c r="G61" s="59"/>
-      <c r="H61" s="59"/>
-      <c r="I61" s="61"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="62"/>
-      <c r="B62" s="63"/>
-      <c r="C62" s="64"/>
-      <c r="D62" s="63"/>
-      <c r="E62" s="63"/>
-      <c r="F62" s="63"/>
-      <c r="G62" s="63"/>
-      <c r="H62" s="63"/>
-      <c r="I62" s="65"/>
+      <c r="A59" s="62"/>
+      <c r="B59" s="63"/>
+      <c r="C59" s="64"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="63"/>
+      <c r="F59" s="63"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="63"/>
+      <c r="I59" s="65"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>